<commit_message>
Deadline changed to 30
</commit_message>
<xml_diff>
--- a/Programming-Basics-Book-Project-Plan.xlsx
+++ b/Programming-Basics-Book-Project-Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20496" windowHeight="9048" tabRatio="306"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20496" windowHeight="9048" tabRatio="306"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Basics Book - Plan" sheetId="1" r:id="rId1"/>
@@ -1671,7 +1671,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>